<commit_message>
Machine Learning on Original Imbalanced Dataset
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aa8172b9163bf4b/Documents/CCT/DataAnalytics/8.Capstone/Capstone Github Repository/MSc-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{8B975B9C-7C3C-4FA1-999B-11F3734BEEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C326C7B-5379-42F9-A060-70C3766B35CB}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{8B975B9C-7C3C-4FA1-999B-11F3734BEEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D7992B0-A35B-4DCB-8D37-E991E65BDA32}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-480" yWindow="804" windowWidth="21600" windowHeight="11232" activeTab="3" xr2:uid="{71125767-81DB-46BD-9156-A0AA2BEEECE0}"/>
+    <workbookView xWindow="29265" yWindow="1665" windowWidth="21600" windowHeight="11235" activeTab="4" xr2:uid="{71125767-81DB-46BD-9156-A0AA2BEEECE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="84">
   <si>
     <t>Comparison</t>
   </si>
@@ -264,6 +265,33 @@
   </si>
   <si>
     <t>Statistical Significance for CommDateProvided:</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>ROC AUC Score</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Gradient Boosting</t>
+  </si>
+  <si>
+    <t>LightGBM</t>
   </si>
 </sst>
 </file>
@@ -343,6 +371,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2586,7 +2618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E57A0E-6596-4AB3-B2A7-58C8B1D5AC8C}">
   <dimension ref="B2:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B51" sqref="B51:E62"/>
     </sheetView>
   </sheetViews>
@@ -3399,4 +3431,146 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E628E468-E23C-4834-ABD1-BF2876B0156E}">
+  <dimension ref="B2:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected Errors in results. Added new visualisations of ML performance
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aa8172b9163bf4b/Documents/CCT/DataAnalytics/8.Capstone/Capstone Github Repository/MSc-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="8_{8B975B9C-7C3C-4FA1-999B-11F3734BEEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A14D298-814C-41B4-8D2A-C92FC2DE47EB}"/>
+  <xr:revisionPtr revIDLastSave="387" documentId="8_{8B975B9C-7C3C-4FA1-999B-11F3734BEEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBCA3482-8BA9-4153-933F-F121B4B6F993}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="34020" yWindow="7155" windowWidth="17280" windowHeight="8880" tabRatio="855" firstSheet="14" activeTab="21" xr2:uid="{71125767-81DB-46BD-9156-A0AA2BEEECE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="855" firstSheet="16" activeTab="21" xr2:uid="{71125767-81DB-46BD-9156-A0AA2BEEECE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Final touches for submission
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aa8172b9163bf4b/Documents/CCT/DataAnalytics/8.Capstone/Capstone Github Repository/MSc-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="387" documentId="8_{8B975B9C-7C3C-4FA1-999B-11F3734BEEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBCA3482-8BA9-4153-933F-F121B4B6F993}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="8_{8B975B9C-7C3C-4FA1-999B-11F3734BEEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D7E189D-C648-48B2-9151-4FE76E973D4A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="855" firstSheet="16" activeTab="21" xr2:uid="{71125767-81DB-46BD-9156-A0AA2BEEECE0}"/>
+    <workbookView minimized="1" xWindow="38820" yWindow="1635" windowWidth="17280" windowHeight="8880" tabRatio="855" firstSheet="16" activeTab="22" xr2:uid="{71125767-81DB-46BD-9156-A0AA2BEEECE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="Oversampled Class Aware" sheetId="14" r:id="rId20"/>
     <sheet name="Oversampled RFECV" sheetId="16" r:id="rId21"/>
     <sheet name="Oversampled Association Analysi" sheetId="17" r:id="rId22"/>
+    <sheet name="Experimentation" sheetId="24" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="204">
   <si>
     <t>Comparison</t>
   </si>
@@ -663,6 +664,12 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Control Accuracy</t>
+  </si>
+  <si>
+    <t>Experiment Accuracy</t>
   </si>
 </sst>
 </file>
@@ -8618,7 +8625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12671294-877D-4CE7-828C-5A01E8BEB8F6}">
   <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E23"/>
     </sheetView>
   </sheetViews>
@@ -8937,6 +8944,1317 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C415F72-93D4-466F-9A50-BC819B9CFD14}">
+  <dimension ref="B2:K59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.75480000000000003</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.69779999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.68430000000000002</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="1">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="10"/>
+      <c r="C4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.77839999999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.78090000000000004</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.76219999999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.7681</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5.7200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="11"/>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.79990000000000006</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.81040000000000001</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.76480000000000004</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.75549999999999995</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.69879999999999998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.2802</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.16259999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
+      <c r="C7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.77739999999999998</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.78280000000000005</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.76190000000000002</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.76780000000000004</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.87180000000000002</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.96109999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="11"/>
+      <c r="C8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.79969999999999997</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.80930000000000002</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="1">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>4.9700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.76380000000000003</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.75980000000000003</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.68810000000000004</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.1196</v>
+      </c>
+      <c r="K9" s="1">
+        <v>4.8899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="10"/>
+      <c r="C10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.77980000000000005</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.76270000000000004</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.76390000000000002</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="1">
+        <v>6.59E-2</v>
+      </c>
+      <c r="K10" s="1">
+        <v>6.4199999999999993E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="11"/>
+      <c r="C11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.80179999999999996</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.81079999999999997</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.12330000000000001</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5.6099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.76390000000000002</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.74139999999999995</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.69769999999999999</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.58879999999999999</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="K12" s="1">
+        <v>6.54E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
+      <c r="C13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.77829999999999999</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.75939999999999996</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.76270000000000004</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.73340000000000005</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="1">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="11"/>
+      <c r="C14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.7833</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.79079999999999995</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2.76E-2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3.27E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.76439999999999997</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.59160000000000001</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.56140000000000001</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="K15" s="1">
+        <v>3.3099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
+      <c r="C16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.7782</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.65720000000000001</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.76239999999999997</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.60009999999999997</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" s="1">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="K16" s="1">
+        <v>5.4899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+      <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.71279999999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.59619999999999995</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K17" s="1">
+        <v>4.9799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.76370000000000005</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.69340000000000002</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="1">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="K18" s="1">
+        <v>5.04E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="10"/>
+      <c r="C19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.77810000000000001</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.77659999999999996</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.7621</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.76180000000000003</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="1">
+        <v>5.21E-2</v>
+      </c>
+      <c r="K19" s="1">
+        <v>4.9599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+      <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.80210000000000004</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="1">
+        <v>6.6100000000000006E-2</v>
+      </c>
+      <c r="K20" s="1">
+        <v>4.36E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.76439999999999997</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.754</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.69740000000000002</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.68340000000000001</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="1">
+        <v>6.0299999999999999E-2</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5.74E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.7772</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.76859999999999995</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.76219999999999999</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.76380000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="11"/>
+      <c r="C23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.80179999999999996</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.81040000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.76039999999999996</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.69269999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
+      <c r="C25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.77710000000000001</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.77510000000000001</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.75590000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.8075</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.76390000000000002</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.71489999999999998</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.69710000000000005</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.66020000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="10"/>
+      <c r="C28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.7772</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.77470000000000006</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.76280000000000003</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.7661</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="11"/>
+      <c r="C29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.80210000000000004</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.81089999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.76380000000000003</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.75319999999999998</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.69769999999999999</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.65739999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="10"/>
+      <c r="C31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.77339999999999998</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.76239999999999997</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.76129999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="11"/>
+      <c r="C32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.79769999999999996</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.80449999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.76329999999999998</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.69740000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="10"/>
+      <c r="C34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.77839999999999998</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.77929999999999999</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.7621</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.76380000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="11"/>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.76370000000000005</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.75739999999999996</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.69689999999999996</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.68520000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="10"/>
+      <c r="C37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.78320000000000001</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.77769999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="11"/>
+      <c r="C38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.76439999999999997</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.6976</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.69189999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="10"/>
+      <c r="C40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.78259999999999996</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.77539999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="11"/>
+      <c r="C41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.80020000000000002</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.81059999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.76439999999999997</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.76229999999999998</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.6986</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.69350000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="10"/>
+      <c r="C43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.77739999999999998</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.77459999999999996</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.76049999999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="11"/>
+      <c r="C44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.76349999999999996</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.76349999999999996</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.69650000000000001</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.69689999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="10"/>
+      <c r="C46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.77859999999999996</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.77859999999999996</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.76329999999999998</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.76290000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="11"/>
+      <c r="C47" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.80189999999999995</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.81110000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.76429999999999998</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.76239999999999997</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.69769999999999999</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.6804</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="10"/>
+      <c r="C49" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.77890000000000004</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.76219999999999999</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.76339999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="11"/>
+      <c r="C50" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.80220000000000002</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.81079999999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.76449999999999996</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.76429999999999998</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.6986</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0.69869999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="10"/>
+      <c r="C52" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.7782</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.7782</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0.76239999999999997</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.76190000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="11"/>
+      <c r="C53" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.76370000000000005</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0.75549999999999995</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0.69740000000000002</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0.68869999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="10"/>
+      <c r="C55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0.77490000000000003</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0.7621</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0.76639999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="11"/>
+      <c r="C56" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0.81069999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0.75980000000000003</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0.69869999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="10"/>
+      <c r="C58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0.77729999999999999</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0.76219999999999999</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0.75749999999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="11"/>
+      <c r="C59" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.80249999999999999</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0.80859999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>